<commit_message>
chore: update components sheet
</commit_message>
<xml_diff>
--- a/Doc/IoT_phases.xlsx
+++ b/Doc/IoT_phases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SMASHBOX\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SMASHBOX\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94A6160-4C78-48ED-BF6D-2DDCB02C67DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057DBD41-8F98-4D8D-88D3-B926EC6F1ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E5DAE876-DA7A-4056-B6BB-BA3A1E2C4B41}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{E5DAE876-DA7A-4056-B6BB-BA3A1E2C4B41}"/>
   </bookViews>
   <sheets>
     <sheet name="PHASES" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>PHASE</t>
   </si>
@@ -235,13 +235,16 @@
   </si>
   <si>
     <t>Questa viene a valle dell'attivita 1,2,3,4</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,7 +408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -434,7 +437,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -467,10 +469,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -808,18 +816,18 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="83.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="83.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" thickBot="1"/>
-    <row r="3" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -833,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42.75">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -847,7 +855,7 @@
         <v>45605</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42.75">
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -861,7 +869,7 @@
         <v>45657</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.5">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -875,7 +883,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -889,7 +897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -906,7 +914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -920,8 +928,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="20"/>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -936,50 +944,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB7CD65-31BA-460D-845D-7C9DD0EF7CC7}">
   <dimension ref="B5:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.875" style="1"/>
+    <col min="4" max="4" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="13">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>2</v>
       </c>
@@ -991,7 +999,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>3</v>
       </c>
@@ -1001,9 +1009,9 @@
       <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="2:5">
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>4</v>
       </c>
@@ -1013,9 +1021,9 @@
       <c r="D10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>5</v>
       </c>
@@ -1025,24 +1033,24 @@
       <c r="D11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="2:5">
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
     </row>
   </sheetData>
@@ -1058,41 +1066,41 @@
   <dimension ref="B5:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="1"/>
+    <col min="6" max="6" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" ht="15" thickBot="1">
+    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>0</v>
       </c>
@@ -1103,22 +1111,22 @@
         <v>6</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="2:6" ht="28.5">
-      <c r="B8" s="13">
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="12">
         <v>1</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="2:6">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>2</v>
       </c>
@@ -1131,7 +1139,7 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>3</v>
       </c>
@@ -1144,7 +1152,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>4</v>
       </c>
@@ -1157,7 +1165,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>5</v>
       </c>
@@ -1172,7 +1180,7 @@
       </c>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>6</v>
       </c>
@@ -1185,13 +1193,13 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
     </row>
   </sheetData>
@@ -1210,53 +1218,53 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" ht="15" thickBot="1">
+    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="13">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>2</v>
       </c>
@@ -1269,7 +1277,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>3</v>
       </c>
@@ -1282,7 +1290,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>4</v>
       </c>
@@ -1295,7 +1303,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>5</v>
       </c>
@@ -1308,7 +1316,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>6</v>
       </c>
@@ -1317,13 +1325,13 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
     </row>
   </sheetData>
@@ -1336,114 +1344,124 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FE4351-B95C-4794-B99C-E4D389725CDF}">
-  <dimension ref="B4:E10"/>
+  <dimension ref="B4:F10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="108.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="108.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" ht="15">
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="2:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="11" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="11" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{C97A6163-B095-4465-BE90-92B2714FEAF0}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{B9BB502F-A9A9-44BF-AD2C-EA6D9CDE39D9}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{12D8B316-FC17-447A-9623-D7B1C617300B}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{DC6C29BB-AA09-49D2-BF83-07F8CD794B3F}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{C97A6163-B095-4465-BE90-92B2714FEAF0}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{B9BB502F-A9A9-44BF-AD2C-EA6D9CDE39D9}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{12D8B316-FC17-447A-9623-D7B1C617300B}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{DC6C29BB-AA09-49D2-BF83-07F8CD794B3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
doc: update TODO documentation and phases files
</commit_message>
<xml_diff>
--- a/Doc/IoT_phases.xlsx
+++ b/Doc/IoT_phases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SMASHBOX\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057DBD41-8F98-4D8D-88D3-B926EC6F1ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0861ACB-64C4-4DF9-B2DE-0BC5F181D318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{E5DAE876-DA7A-4056-B6BB-BA3A1E2C4B41}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
   <si>
     <t>PHASE</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Fre (?)</t>
-  </si>
-  <si>
     <t>Software e HW design</t>
   </si>
   <si>
@@ -238,6 +235,15 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Fre/Simo</t>
+  </si>
+  <si>
+    <t>Dare script di test per pacchetto monitoring</t>
+  </si>
+  <si>
+    <t>Arduino Uno</t>
   </si>
 </sst>
 </file>
@@ -874,7 +880,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
@@ -945,7 +951,7 @@
   <dimension ref="B5:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,26 +991,26 @@
       <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="9"/>
+        <v>59</v>
+      </c>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>6</v>
@@ -1016,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>6</v>
@@ -1063,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE7C5B0-DBCA-4CB4-8E65-FFC605021D87}">
-  <dimension ref="B5:F16"/>
+  <dimension ref="B5:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,7 +1081,7 @@
     <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1105,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>6</v>
@@ -1118,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>22</v>
@@ -1131,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>22</v>
@@ -1140,11 +1146,11 @@
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="7">
+      <c r="B10" s="12">
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>6</v>
@@ -1156,51 +1162,64 @@
       <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>63</v>
+      <c r="C11" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="7">
+      <c r="B12" s="12">
         <v>5</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>47</v>
+      <c r="C12" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="2"/>
+      <c r="B14" s="12">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1254,13 +1273,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="14"/>
     </row>
@@ -1269,7 +1288,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>22</v>
@@ -1282,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>6</v>
@@ -1295,7 +1314,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>6</v>
@@ -1308,7 +1327,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>22</v>
@@ -1344,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FE4351-B95C-4794-B99C-E4D389725CDF}">
-  <dimension ref="B4:F10"/>
+  <dimension ref="B4:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1364,7 +1383,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>27</v>
@@ -1443,16 +1462,27 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1462,6 +1492,7 @@
     <hyperlink ref="D7" r:id="rId2" xr:uid="{B9BB502F-A9A9-44BF-AD2C-EA6D9CDE39D9}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{12D8B316-FC17-447A-9623-D7B1C617300B}"/>
     <hyperlink ref="D8" r:id="rId4" xr:uid="{DC6C29BB-AA09-49D2-BF83-07F8CD794B3F}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{9CF69C5F-9F6A-47EE-B79A-1EBFB358D19A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
doc: update documentation on different files
</commit_message>
<xml_diff>
--- a/Doc/IoT_phases.xlsx
+++ b/Doc/IoT_phases.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SMASHBOX\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C07215-283C-4175-BD67-B3441EE33BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="23256" windowHeight="13176" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHASES" sheetId="1" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="ALPHA 2" sheetId="8" r:id="rId4"/>
     <sheet name="Componenti" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -246,8 +252,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,7 +300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -406,23 +412,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,7 +484,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -817,32 +811,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="1"/>
-    <col min="2" max="2" width="83.8984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="83.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" thickBot="1"/>
-    <row r="3" spans="1:5" ht="14.4">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -856,7 +850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -870,7 +864,7 @@
         <v>45605</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="41.4">
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -884,7 +878,7 @@
         <v>45657</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="27.6">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -898,7 +892,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -912,7 +906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -929,7 +923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -943,7 +937,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="19"/>
     </row>
   </sheetData>
@@ -956,27 +950,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B5:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="1"/>
-    <col min="2" max="2" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.8984375" style="1"/>
+    <col min="4" max="4" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" ht="15" thickBot="1">
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1">
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
@@ -990,7 +984,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="14.4">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>1</v>
       </c>
@@ -1002,7 +996,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="2:5" ht="14.4">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>2</v>
       </c>
@@ -1014,7 +1008,7 @@
       </c>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:5" ht="14.4">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>3</v>
       </c>
@@ -1026,7 +1020,7 @@
       </c>
       <c r="E9" s="20"/>
     </row>
-    <row r="10" spans="2:5" ht="14.4">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>4</v>
       </c>
@@ -1038,7 +1032,7 @@
       </c>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="2:5" ht="14.4">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>5</v>
       </c>
@@ -1050,22 +1044,22 @@
       </c>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="2:5" ht="14.4">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="2:5" ht="14.4">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:5" ht="14.4">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:5" ht="14.4">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:5" ht="14.4">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
     </row>
   </sheetData>
@@ -1077,28 +1071,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="1"/>
-    <col min="2" max="2" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" ht="15" thickBot="1">
+    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:6" ht="15" thickBot="1">
+    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
@@ -1115,7 +1109,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="14.4">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>0</v>
       </c>
@@ -1128,7 +1122,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="2:6" ht="28.8">
+    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>1</v>
       </c>
@@ -1141,7 +1135,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="2:6" ht="14.4">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>2</v>
       </c>
@@ -1154,7 +1148,7 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="2:6" ht="14.4">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="12">
         <v>3</v>
       </c>
@@ -1167,7 +1161,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="2:6" ht="14.4">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>4</v>
       </c>
@@ -1178,9 +1172,9 @@
         <v>6</v>
       </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="2:6" ht="14.4">
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
         <v>5</v>
       </c>
@@ -1193,7 +1187,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" ht="14.4">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>6</v>
       </c>
@@ -1208,7 +1202,7 @@
       </c>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
         <v>7</v>
       </c>
@@ -1221,13 +1215,13 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" ht="14.4">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:6" ht="14.4">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="3:3" ht="14.4">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
     </row>
   </sheetData>
@@ -1239,28 +1233,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B5:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="1"/>
-    <col min="2" max="2" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" ht="15" thickBot="1">
+    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:6" ht="15" thickBot="1">
+    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
@@ -1277,7 +1271,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>1</v>
       </c>
@@ -1292,7 +1286,7 @@
       </c>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>2</v>
       </c>
@@ -1305,7 +1299,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="2:6" ht="14.4">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>3</v>
       </c>
@@ -1318,7 +1312,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="14.4">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>4</v>
       </c>
@@ -1331,7 +1325,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="2:6" ht="14.4">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>5</v>
       </c>
@@ -1344,7 +1338,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" ht="14.4">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>6</v>
       </c>
@@ -1353,13 +1347,13 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="14" spans="2:6" ht="14.4">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:6" ht="14.4">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:6" ht="14.4">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
     </row>
   </sheetData>
@@ -1371,23 +1365,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B4:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="108.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="108.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" s="23" customFormat="1" ht="14.4">
+    <row r="4" spans="2:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="22" t="s">
         <v>26</v>
       </c>
@@ -1404,7 +1398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
@@ -1419,7 +1413,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="14.4">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>29</v>
       </c>
@@ -1432,7 +1426,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
@@ -1447,7 +1441,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>33</v>
       </c>
@@ -1462,7 +1456,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="14.4">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>34</v>
       </c>
@@ -1477,7 +1471,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="14.4">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>67</v>
       </c>
@@ -1490,7 +1484,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="2:6" ht="14.4">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>38</v>
       </c>
@@ -1505,22 +1499,25 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="24" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="10">
         <f>SUM(C5:C11)</f>
         <v>72.52</v>
       </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D7" r:id="rId2"/>
-    <hyperlink ref="D6" r:id="rId3"/>
-    <hyperlink ref="D8" r:id="rId4"/>
-    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
chore: update development phases
</commit_message>
<xml_diff>
--- a/Doc/IoT_phases.xlsx
+++ b/Doc/IoT_phases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SMASHBOX\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C07215-283C-4175-BD67-B3441EE33BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E7684D-8427-4D00-9F46-894659C1CC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHASES" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
   <si>
     <t>PHASE</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>TOTALE:</t>
+  </si>
+  <si>
+    <t>Attività terminata, verifichiamo se ottenere un ID da poter salvare in cloud</t>
+  </si>
+  <si>
+    <t>Gestione database per Customers</t>
+  </si>
+  <si>
+    <t>Verificare autoriconoscimento porte seriali</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1084,7 @@
   <dimension ref="B5:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,7 +1093,7 @@
     <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1133,7 +1142,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
@@ -1145,8 +1154,10 @@
       <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="12">
@@ -1185,7 +1196,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
@@ -1216,10 +1227,30 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="2"/>
+      <c r="B15" s="12">
+        <v>8</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="2"/>
+      <c r="B16" s="12">
+        <v>9</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
@@ -1237,7 +1268,7 @@
   <dimension ref="B5:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
doc: update completed phases on Alpha 1
</commit_message>
<xml_diff>
--- a/Doc/IoT_phases.xlsx
+++ b/Doc/IoT_phases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SMASHBOX\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDFE62F-E448-442C-9981-E64985E057BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C424C33-37B8-4ECE-AA99-978C163FE0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHASES" sheetId="1" r:id="rId1"/>
@@ -255,10 +255,10 @@
     <t>Gestione database per Customers</t>
   </si>
   <si>
-    <t>Comunicazione multipla Central/Acquisition Bridge</t>
-  </si>
-  <si>
     <t>Da verificare se ne vale la pena</t>
+  </si>
+  <si>
+    <t>Autorecognition serial</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,7 +1173,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
@@ -1214,7 +1214,7 @@
       <c r="E13" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
@@ -1227,7 +1227,7 @@
         <v>65</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
@@ -1247,7 +1247,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>6</v>
@@ -1270,7 +1270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B5:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1370,7 +1370,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="7"/>
     </row>

</xml_diff>

<commit_message>
doc: end Alpha 1 and update Alpha 2 phases
</commit_message>
<xml_diff>
--- a/Doc/IoT_phases.xlsx
+++ b/Doc/IoT_phases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SMASHBOX\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C424C33-37B8-4ECE-AA99-978C163FE0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81D1E45-B875-4FD2-9510-5028DD2CED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHASES" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
   <si>
     <t>PHASE</t>
   </si>
@@ -192,18 +192,12 @@
     <t>Inizializzare repo progetto su Git</t>
   </si>
   <si>
-    <t>Da valutare la situazione una volta chiuso Alpha-1</t>
-  </si>
-  <si>
     <t>Ordine componenti Amazon</t>
   </si>
   <si>
     <t>Fattibilità  per comunicazioni Client-Cloud</t>
   </si>
   <si>
-    <t>Risoluzione criticità</t>
-  </si>
-  <si>
     <t>Verificare la possibilità di inviare dati wireless</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>TOTALE:</t>
   </si>
   <si>
-    <t>Attività terminata, verifichiamo se ottenere un ID da poter salvare in cloud</t>
-  </si>
-  <si>
     <t>Gestione database per Customers</t>
   </si>
   <si>
@@ -259,6 +250,21 @@
   </si>
   <si>
     <t>Autorecognition serial</t>
+  </si>
+  <si>
+    <t>Simulazione di più box sullo stesso bridge</t>
+  </si>
+  <si>
+    <t>ClientServer(Bot Telegram?) per visualizzare log accessi?</t>
+  </si>
+  <si>
+    <t>Dubbi</t>
+  </si>
+  <si>
+    <t>Central: due sketch: train + main?</t>
+  </si>
+  <si>
+    <t>Local: uno sketch?</t>
   </si>
 </sst>
 </file>
@@ -895,7 +901,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
@@ -1013,10 +1019,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" s="21"/>
     </row>
@@ -1086,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>22</v>
@@ -1157,9 +1163,7 @@
       <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="E9" s="9"/>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -1167,7 +1171,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>6</v>
@@ -1180,7 +1184,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>6</v>
@@ -1193,7 +1197,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>6</v>
@@ -1212,7 +1216,7 @@
         <v>47</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F13" s="21"/>
     </row>
@@ -1221,10 +1225,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="21"/>
@@ -1234,7 +1238,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>6</v>
@@ -1247,13 +1251,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
@@ -1268,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B5:F16"/>
+  <dimension ref="B5:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,14 +1314,12 @@
         <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -1325,7 +1327,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>22</v>
@@ -1338,10 +1340,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1351,7 +1353,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>6</v>
@@ -1364,13 +1366,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" s="7"/>
     </row>
@@ -1378,8 +1380,12 @@
       <c r="B12" s="7">
         <v>6</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
@@ -1387,10 +1393,22 @@
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1422,7 +1440,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>27</v>
@@ -1509,13 +1527,13 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="10">
         <v>28.5</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -1537,7 +1555,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" s="10">
         <f>SUM(C5:C11)</f>

</xml_diff>